<commit_message>
tried new parameters: segment size = 10
</commit_message>
<xml_diff>
--- a/apgar1unhealthy.xlsx
+++ b/apgar1unhealthy.xlsx
@@ -476,22 +476,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=30.008368232866097)</t>
+          <t>ReturnTuple(sdnn=29.871379591073207)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=30.008368232866097)</t>
+          <t>ReturnTuple(sdnn=29.871379591073207)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=30.008368232866097)</t>
+          <t>ReturnTuple(sdnn=29.871379591073207)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=30.008368232866097)</t>
+          <t>ReturnTuple(sdnn=29.871379591073207)</t>
         </is>
       </c>
     </row>
@@ -506,22 +506,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=23.98278428923992)</t>
+          <t>ReturnTuple(sdnn=23.734258537001377)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=23.98278428923992)</t>
+          <t>ReturnTuple(sdnn=23.734258537001377)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=23.98278428923992)</t>
+          <t>ReturnTuple(sdnn=23.734258537001377)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=23.98278428923992)</t>
+          <t>ReturnTuple(sdnn=23.734258537001377)</t>
         </is>
       </c>
     </row>
@@ -536,22 +536,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=20.447303227431547)</t>
+          <t>ReturnTuple(sdnn=19.9648155496385)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=20.447303227431547)</t>
+          <t>ReturnTuple(sdnn=19.9648155496385)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=20.447303227431547)</t>
+          <t>ReturnTuple(sdnn=19.9648155496385)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=20.447303227431547)</t>
+          <t>ReturnTuple(sdnn=19.9648155496385)</t>
         </is>
       </c>
     </row>
@@ -566,22 +566,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.592306580238088)</t>
+          <t>ReturnTuple(sdnn=18.628600778943706)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.592306580238088)</t>
+          <t>ReturnTuple(sdnn=18.628600778943706)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.592306580238088)</t>
+          <t>ReturnTuple(sdnn=18.628600778943706)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.592306580238088)</t>
+          <t>ReturnTuple(sdnn=18.628600778943706)</t>
         </is>
       </c>
     </row>
@@ -596,22 +596,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.61615156217473)</t>
+          <t>ReturnTuple(sdnn=16.2790493823268)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.61615156217473)</t>
+          <t>ReturnTuple(sdnn=16.2790493823268)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.61615156217473)</t>
+          <t>ReturnTuple(sdnn=16.2790493823268)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.61615156217473)</t>
+          <t>ReturnTuple(sdnn=16.2790493823268)</t>
         </is>
       </c>
     </row>
@@ -626,22 +626,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.160599650051903)</t>
+          <t>ReturnTuple(sdnn=19.046189094326152)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.160599650051903)</t>
+          <t>ReturnTuple(sdnn=19.046189094326152)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.160599650051903)</t>
+          <t>ReturnTuple(sdnn=19.046189094326152)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.160599650051903)</t>
+          <t>ReturnTuple(sdnn=19.046189094326152)</t>
         </is>
       </c>
     </row>
@@ -656,22 +656,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.89328268712506)</t>
+          <t>ReturnTuple(sdnn=18.466857897712615)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.89328268712506)</t>
+          <t>ReturnTuple(sdnn=18.466857897712615)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.89328268712506)</t>
+          <t>ReturnTuple(sdnn=18.466857897712615)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.89328268712506)</t>
+          <t>ReturnTuple(sdnn=18.466857897712615)</t>
         </is>
       </c>
     </row>
@@ -686,22 +686,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.410953484240004)</t>
+          <t>ReturnTuple(sdnn=21.45385155342088)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.410953484240004)</t>
+          <t>ReturnTuple(sdnn=21.45385155342088)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.410953484240004)</t>
+          <t>ReturnTuple(sdnn=21.45385155342088)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.410953484240004)</t>
+          <t>ReturnTuple(sdnn=21.45385155342088)</t>
         </is>
       </c>
     </row>
@@ -716,22 +716,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=22.34690942869585)</t>
+          <t>ReturnTuple(sdnn=22.204304741127483)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=22.34690942869585)</t>
+          <t>ReturnTuple(sdnn=22.204304741127483)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=22.34690942869585)</t>
+          <t>ReturnTuple(sdnn=22.204304741127483)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=22.34690942869585)</t>
+          <t>ReturnTuple(sdnn=22.204304741127483)</t>
         </is>
       </c>
     </row>
@@ -746,22 +746,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.21992532478053)</t>
+          <t>ReturnTuple(sdnn=18.06993412458282)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.21992532478053)</t>
+          <t>ReturnTuple(sdnn=18.06993412458282)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.21992532478053)</t>
+          <t>ReturnTuple(sdnn=18.06993412458282)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=18.21992532478053)</t>
+          <t>ReturnTuple(sdnn=18.06993412458282)</t>
         </is>
       </c>
     </row>
@@ -776,22 +776,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=15.512508219000823)</t>
+          <t>ReturnTuple(sdnn=15.48470001172583)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=15.512508219000823)</t>
+          <t>ReturnTuple(sdnn=15.48470001172583)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=15.512508219000823)</t>
+          <t>ReturnTuple(sdnn=15.48470001172583)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=15.512508219000823)</t>
+          <t>ReturnTuple(sdnn=15.48470001172583)</t>
         </is>
       </c>
     </row>
@@ -806,22 +806,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.423296877853204)</t>
+          <t>ReturnTuple(sdnn=16.336820679251357)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.423296877853204)</t>
+          <t>ReturnTuple(sdnn=16.336820679251357)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.423296877853204)</t>
+          <t>ReturnTuple(sdnn=16.336820679251357)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.423296877853204)</t>
+          <t>ReturnTuple(sdnn=16.336820679251357)</t>
         </is>
       </c>
     </row>
@@ -836,22 +836,22 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.313080658347655)</t>
+          <t>ReturnTuple(sdnn=21.267563599808607)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.313080658347655)</t>
+          <t>ReturnTuple(sdnn=21.267563599808607)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.313080658347655)</t>
+          <t>ReturnTuple(sdnn=21.267563599808607)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.313080658347655)</t>
+          <t>ReturnTuple(sdnn=21.267563599808607)</t>
         </is>
       </c>
     </row>
@@ -866,22 +866,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=20.130789472725528)</t>
+          <t>ReturnTuple(sdnn=19.996736627512522)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=20.130789472725528)</t>
+          <t>ReturnTuple(sdnn=19.996736627512522)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=20.130789472725528)</t>
+          <t>ReturnTuple(sdnn=19.996736627512522)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=20.130789472725528)</t>
+          <t>ReturnTuple(sdnn=19.996736627512522)</t>
         </is>
       </c>
     </row>
@@ -896,22 +896,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=10.6888504778175)</t>
+          <t>ReturnTuple(sdnn=10.676169148366048)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=10.6888504778175)</t>
+          <t>ReturnTuple(sdnn=10.676169148366048)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=10.6888504778175)</t>
+          <t>ReturnTuple(sdnn=10.676169148366048)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=10.6888504778175)</t>
+          <t>ReturnTuple(sdnn=10.676169148366048)</t>
         </is>
       </c>
     </row>
@@ -926,22 +926,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=24.445709191303635)</t>
+          <t>ReturnTuple(sdnn=24.44593306808824)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=24.445709191303635)</t>
+          <t>ReturnTuple(sdnn=24.44593306808824)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=24.445709191303635)</t>
+          <t>ReturnTuple(sdnn=24.44593306808824)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=24.445709191303635)</t>
+          <t>ReturnTuple(sdnn=24.44593306808824)</t>
         </is>
       </c>
     </row>
@@ -956,22 +956,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=12.858714145687314)</t>
+          <t>ReturnTuple(sdnn=12.300549447255673)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=12.858714145687314)</t>
+          <t>ReturnTuple(sdnn=12.300549447255673)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=12.858714145687314)</t>
+          <t>ReturnTuple(sdnn=12.300549447255673)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=12.858714145687314)</t>
+          <t>ReturnTuple(sdnn=12.300549447255673)</t>
         </is>
       </c>
     </row>
@@ -986,22 +986,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.409912504455278)</t>
+          <t>ReturnTuple(sdnn=19.109729235928555)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.409912504455278)</t>
+          <t>ReturnTuple(sdnn=19.109729235928555)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.409912504455278)</t>
+          <t>ReturnTuple(sdnn=19.109729235928555)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.409912504455278)</t>
+          <t>ReturnTuple(sdnn=19.109729235928555)</t>
         </is>
       </c>
     </row>
@@ -1016,22 +1016,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=15.68138189737738)</t>
+          <t>ReturnTuple(sdnn=15.36459887606487)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=15.68138189737738)</t>
+          <t>ReturnTuple(sdnn=15.36459887606487)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=15.68138189737738)</t>
+          <t>ReturnTuple(sdnn=15.36459887606487)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=15.68138189737738)</t>
+          <t>ReturnTuple(sdnn=15.36459887606487)</t>
         </is>
       </c>
     </row>
@@ -1046,22 +1046,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.125955059164806)</t>
+          <t>ReturnTuple(sdnn=19.160646719617016)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.125955059164806)</t>
+          <t>ReturnTuple(sdnn=19.160646719617016)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.125955059164806)</t>
+          <t>ReturnTuple(sdnn=19.160646719617016)</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=19.125955059164806)</t>
+          <t>ReturnTuple(sdnn=19.160646719617016)</t>
         </is>
       </c>
     </row>
@@ -1076,22 +1076,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=14.656439003174677)</t>
+          <t>ReturnTuple(sdnn=14.481527814310157)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=14.656439003174677)</t>
+          <t>ReturnTuple(sdnn=14.481527814310157)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=14.656439003174677)</t>
+          <t>ReturnTuple(sdnn=14.481527814310157)</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=14.656439003174677)</t>
+          <t>ReturnTuple(sdnn=14.481527814310157)</t>
         </is>
       </c>
     </row>
@@ -1106,22 +1106,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=17.49863514094865)</t>
+          <t>ReturnTuple(sdnn=17.20350490714225)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=17.49863514094865)</t>
+          <t>ReturnTuple(sdnn=17.20350490714225)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=17.49863514094865)</t>
+          <t>ReturnTuple(sdnn=17.20350490714225)</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=17.49863514094865)</t>
+          <t>ReturnTuple(sdnn=17.20350490714225)</t>
         </is>
       </c>
     </row>
@@ -1136,22 +1136,22 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.242656003421857)</t>
+          <t>ReturnTuple(sdnn=16.24465216380139)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.242656003421857)</t>
+          <t>ReturnTuple(sdnn=16.24465216380139)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.242656003421857)</t>
+          <t>ReturnTuple(sdnn=16.24465216380139)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=16.242656003421857)</t>
+          <t>ReturnTuple(sdnn=16.24465216380139)</t>
         </is>
       </c>
     </row>
@@ -1166,22 +1166,22 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.614200821420216)</t>
+          <t>ReturnTuple(sdnn=21.623741553475075)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.614200821420216)</t>
+          <t>ReturnTuple(sdnn=21.623741553475075)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.614200821420216)</t>
+          <t>ReturnTuple(sdnn=21.623741553475075)</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.614200821420216)</t>
+          <t>ReturnTuple(sdnn=21.623741553475075)</t>
         </is>
       </c>
     </row>
@@ -1196,22 +1196,22 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.735226020817024)</t>
+          <t>ReturnTuple(sdnn=21.43284376748338)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.735226020817024)</t>
+          <t>ReturnTuple(sdnn=21.43284376748338)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.735226020817024)</t>
+          <t>ReturnTuple(sdnn=21.43284376748338)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=21.735226020817024)</t>
+          <t>ReturnTuple(sdnn=21.43284376748338)</t>
         </is>
       </c>
     </row>
@@ -1226,22 +1226,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=23.060939412020737)</t>
+          <t>ReturnTuple(sdnn=22.421531578161254)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=23.060939412020737)</t>
+          <t>ReturnTuple(sdnn=22.421531578161254)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=23.060939412020737)</t>
+          <t>ReturnTuple(sdnn=22.421531578161254)</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=23.060939412020737)</t>
+          <t>ReturnTuple(sdnn=22.421531578161254)</t>
         </is>
       </c>
     </row>
@@ -1256,22 +1256,22 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=14.626280587125782)</t>
+          <t>ReturnTuple(sdnn=14.521597979402125)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=14.626280587125782)</t>
+          <t>ReturnTuple(sdnn=14.521597979402125)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=14.626280587125782)</t>
+          <t>ReturnTuple(sdnn=14.521597979402125)</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>ReturnTuple(sdnn=14.626280587125782)</t>
+          <t>ReturnTuple(sdnn=14.521597979402125)</t>
         </is>
       </c>
     </row>

</xml_diff>